<commit_message>
Created dictionary with predefined names (English - Bulgarian), set logic to use dictionary, if name not found use transliteration rules
</commit_message>
<xml_diff>
--- a/NameTransliterator.Services/Data/Database Tables (including data).xlsx
+++ b/NameTransliterator.Services/Data/Database Tables (including data).xlsx
@@ -3290,7 +3290,7 @@
     <t>c</t>
   </si>
   <si>
-    <t>NameTransliterationDictionary (Source: BehindTheNames.com)</t>
+    <t>NameTransliterationDictionary</t>
   </si>
 </sst>
 </file>
@@ -3673,8 +3673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H535"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A509" workbookViewId="0">
-      <selection activeCell="C521" sqref="C521"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>